<commit_message>
edit full watchlist set starting day to 20.03.2022
</commit_message>
<xml_diff>
--- a/Full_Watchlist.xlsx
+++ b/Full_Watchlist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\10_Projects\03_Python_Finance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA781451-AA89-4B39-B111-DDC6AD9FD747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F194418C-78C8-4A98-8E1D-947017266C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="828" yWindow="408" windowWidth="11508" windowHeight="9156" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="134">
   <si>
     <t>Symbol</t>
   </si>
@@ -51,21 +51,6 @@
     <t>AAPL</t>
   </si>
   <si>
-    <t>USOIL</t>
-  </si>
-  <si>
-    <t>SILVER</t>
-  </si>
-  <si>
-    <t>GOLD</t>
-  </si>
-  <si>
-    <t>BTCUSD</t>
-  </si>
-  <si>
-    <t>LINKUSD</t>
-  </si>
-  <si>
     <t>CRM</t>
   </si>
   <si>
@@ -337,6 +322,111 @@
   </si>
   <si>
     <t>MRK</t>
+  </si>
+  <si>
+    <t>CAN</t>
+  </si>
+  <si>
+    <t>HES</t>
+  </si>
+  <si>
+    <t>MOS</t>
+  </si>
+  <si>
+    <t>DWAC</t>
+  </si>
+  <si>
+    <t>OKE</t>
+  </si>
+  <si>
+    <t>NTR</t>
+  </si>
+  <si>
+    <t>CMC</t>
+  </si>
+  <si>
+    <t>WHD</t>
+  </si>
+  <si>
+    <t>ORLY</t>
+  </si>
+  <si>
+    <t>GFI</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>OXY</t>
+  </si>
+  <si>
+    <t>ANTM</t>
+  </si>
+  <si>
+    <t>REGN</t>
+  </si>
+  <si>
+    <t>COST</t>
+  </si>
+  <si>
+    <t>JBHT</t>
+  </si>
+  <si>
+    <t>UNH</t>
+  </si>
+  <si>
+    <t>HRMY</t>
+  </si>
+  <si>
+    <t>IRM</t>
+  </si>
+  <si>
+    <t>ODFL</t>
+  </si>
+  <si>
+    <t>AVGO</t>
+  </si>
+  <si>
+    <t>CVS</t>
+  </si>
+  <si>
+    <t>SHELL</t>
+  </si>
+  <si>
+    <t>BRO</t>
+  </si>
+  <si>
+    <t>MAR</t>
+  </si>
+  <si>
+    <t>JNPR</t>
+  </si>
+  <si>
+    <t>MET</t>
+  </si>
+  <si>
+    <t>XOM</t>
+  </si>
+  <si>
+    <t>DKNG</t>
+  </si>
+  <si>
+    <t>COP</t>
+  </si>
+  <si>
+    <t>FDX</t>
+  </si>
+  <si>
+    <t>KBH</t>
+  </si>
+  <si>
+    <t>TMST</t>
+  </si>
+  <si>
+    <t>SSRM</t>
+  </si>
+  <si>
+    <t>ACLS</t>
   </si>
 </sst>
 </file>
@@ -654,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A104"/>
+  <dimension ref="A1:A137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A105" sqref="A105"/>
+    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="A138" sqref="A138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -674,32 +764,32 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
@@ -709,32 +799,32 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
@@ -769,32 +859,32 @@
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
@@ -944,32 +1034,32 @@
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
@@ -1089,32 +1179,32 @@
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>87</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
@@ -1139,32 +1229,32 @@
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>96</v>
+        <v>6</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>6</v>
+        <v>100</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
@@ -1180,6 +1270,171 @@
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>